<commit_message>
revision 1 result and manuscript updated
</commit_message>
<xml_diff>
--- a/result/Table 1.xlsx
+++ b/result/Table 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2020_04_Norah_scFEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalgh\Desktop\Thesis\zitu files\Dr.ChiCode\scFEA_Resubmition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11D666B2-65EB-4CF1-B70F-F172C91F4520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803352B6-D403-4456-9BDD-E135B33A05A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D59EFB9-28B3-41AE-B2CD-D8E170BDE932}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D59EFB9-28B3-41AE-B2CD-D8E170BDE932}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Super Module class</t>
   </si>
@@ -113,17 +113,20 @@
   <si>
     <t>Table 1: Super metabolic module information</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steroid hormone synthesis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -132,7 +135,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -140,14 +143,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,7 +159,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -204,7 +207,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -218,6 +221,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,21 +546,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51588530-D63E-41B8-957B-7372FEF47AAD}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -562,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -576,7 +590,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -590,7 +604,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -604,7 +618,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -618,7 +632,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -632,7 +646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -646,7 +660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -660,7 +674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -674,7 +688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -688,7 +702,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -702,7 +716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -716,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -730,7 +744,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -738,13 +752,13 @@
         <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -758,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -766,13 +780,13 @@
         <v>17</v>
       </c>
       <c r="C17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -780,13 +794,13 @@
         <v>18</v>
       </c>
       <c r="C18" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -794,13 +808,13 @@
         <v>19</v>
       </c>
       <c r="C19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -808,13 +822,13 @@
         <v>20</v>
       </c>
       <c r="C20" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -828,7 +842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -842,18 +856,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:4" s="6" customFormat="1">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="5">
         <v>17</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="5">
         <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="7" customFormat="1" ht="15" thickBot="1">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>